<commit_message>
add reading list and burgers
</commit_message>
<xml_diff>
--- a/Eat_Data.xlsx
+++ b/Eat_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobford/Documents/GitHub/Blog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobford/Documents/GitHub/Writes_and_Wrongs/writes_and_wrongs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5A8699-E397-A340-8809-DB716585C60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4449F8DA-F350-5340-B45D-49949E6C286E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="18660" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>BBQ New Orleans Style Shrimp + Ceviche</t>
+  </si>
+  <si>
+    <t>Neuse River Brewing</t>
+  </si>
+  <si>
+    <t>Neuse River Burger</t>
+  </si>
+  <si>
+    <t>Brassiere/Burgers</t>
   </si>
 </sst>
 </file>
@@ -613,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:F27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1167,6 +1176,26 @@
         <v>-78.647649510751805</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28">
+        <v>35.804566959442603</v>
+      </c>
+      <c r="F28">
+        <v>-78.632520307935593</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>